<commit_message>
Updates for existing Test Cases
</commit_message>
<xml_diff>
--- a/src/test/resources/BMI_CateGory_Name.xlsx
+++ b/src/test/resources/BMI_CateGory_Name.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="28620" windowHeight="12660"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="19440" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,9 +183,6 @@
     <t>INFRASTRUCTURE R/R INDEX</t>
   </si>
   <si>
-    <t>PROJECT FINANCE RATING</t>
-  </si>
-  <si>
     <t>CEMENT</t>
   </si>
   <si>
@@ -201,9 +198,6 @@
     <t>CPI BREAKDOWN</t>
   </si>
   <si>
-    <t>CPI  WEIGHTS</t>
-  </si>
-  <si>
     <t>TOTAL HOUSEHOLD SPENDING</t>
   </si>
   <si>
@@ -844,6 +838,12 @@
   </si>
   <si>
     <t>BMI_10167</t>
+  </si>
+  <si>
+    <t>CPI WEIGHTS</t>
+  </si>
+  <si>
+    <t>PROJECT RISK INDEX</t>
   </si>
 </sst>
 </file>
@@ -1213,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="R89" sqref="R89"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,7 +1226,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1234,7 +1234,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1242,7 +1242,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -1250,7 +1250,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -1258,7 +1258,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -1266,7 +1266,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -1274,7 +1274,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1282,7 +1282,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -1290,7 +1290,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -1306,7 +1306,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -1314,7 +1314,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -1322,7 +1322,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
@@ -1330,7 +1330,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
@@ -1338,7 +1338,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
@@ -1346,7 +1346,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -1354,7 +1354,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
@@ -1362,7 +1362,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
@@ -1370,7 +1370,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
@@ -1378,7 +1378,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
@@ -1386,7 +1386,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
@@ -1394,7 +1394,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
@@ -1402,7 +1402,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
@@ -1410,7 +1410,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
@@ -1418,7 +1418,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
@@ -1426,7 +1426,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
@@ -1442,7 +1442,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
@@ -1450,7 +1450,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
@@ -1458,7 +1458,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
@@ -1466,7 +1466,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
@@ -1474,7 +1474,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
@@ -1482,7 +1482,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
@@ -1490,7 +1490,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B34" t="s">
         <v>33</v>
@@ -1498,7 +1498,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B35" t="s">
         <v>34</v>
@@ -1506,7 +1506,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
@@ -1514,7 +1514,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B37" t="s">
         <v>36</v>
@@ -1522,7 +1522,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B38" t="s">
         <v>37</v>
@@ -1530,7 +1530,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B39" t="s">
         <v>38</v>
@@ -1538,7 +1538,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B40" t="s">
         <v>39</v>
@@ -1546,7 +1546,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B41" t="s">
         <v>40</v>
@@ -1554,7 +1554,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B42" t="s">
         <v>41</v>
@@ -1562,7 +1562,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B43" t="s">
         <v>42</v>
@@ -1570,7 +1570,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B44" t="s">
         <v>43</v>
@@ -1578,7 +1578,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B45" t="s">
         <v>44</v>
@@ -1586,7 +1586,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B46" t="s">
         <v>45</v>
@@ -1594,7 +1594,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B47" t="s">
         <v>46</v>
@@ -1602,7 +1602,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B48" t="s">
         <v>47</v>
@@ -1610,7 +1610,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B49" t="s">
         <v>48</v>
@@ -1618,7 +1618,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B50" t="s">
         <v>49</v>
@@ -1626,7 +1626,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B51" t="s">
         <v>50</v>
@@ -1634,7 +1634,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B52" t="s">
         <v>51</v>
@@ -1642,7 +1642,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B53" t="s">
         <v>52</v>
@@ -1650,7 +1650,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B54" t="s">
         <v>53</v>
@@ -1658,7 +1658,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B55" t="s">
         <v>54</v>
@@ -1666,658 +1666,658 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B56" t="s">
-        <v>55</v>
+        <v>275</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B62" t="s">
-        <v>61</v>
+        <v>274</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B63" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B64" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B65" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B66" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B67" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B68" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B69" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B70" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B71" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B72" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B73" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B74" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B75" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B76" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B77" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B78" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B79" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B80" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B81" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B82" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B83" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B84" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B85" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B86" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B87" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B88" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B89" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B90" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B91" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B92" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B93" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B94" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B95" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B96" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B97" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B98" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B99" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B100" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B101" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B102" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B103" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B104" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B105" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B106" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B107" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B108" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B109" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B110" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B111" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B112" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B113" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B114" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B115" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B116" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B117" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B118" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B119" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B120" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B121" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B122" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B123" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B124" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B125" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B126" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B127" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B128" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B129" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B130" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B131" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B132" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B133" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B134" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B135" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B136" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B137" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2337,10 +2337,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated cds metadat,updated bmi category name
</commit_message>
<xml_diff>
--- a/src/test/resources/BMI_CateGory_Name.xlsx
+++ b/src/test/resources/BMI_CateGory_Name.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="272">
   <si>
     <t>Name</t>
   </si>
@@ -417,9 +417,6 @@
     <t>BMI_10146</t>
   </si>
   <si>
-    <t>BMI_10147</t>
-  </si>
-  <si>
     <t>BMI_10148</t>
   </si>
   <si>
@@ -820,9 +817,6 @@
   </si>
   <si>
     <t>Prices</t>
-  </si>
-  <si>
-    <t>Milk</t>
   </si>
   <si>
     <t>Wheat</t>
@@ -1205,10 +1199,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B136"/>
+  <dimension ref="A1:B135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="A137" sqref="A137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,7 +1226,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1240,7 +1234,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1248,7 +1242,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1256,7 +1250,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1264,7 +1258,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1272,7 +1266,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1280,7 +1274,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1288,7 +1282,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1296,7 +1290,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1304,7 +1298,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1312,7 +1306,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1320,7 +1314,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1328,7 +1322,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1336,7 +1330,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1344,7 +1338,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1352,7 +1346,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1360,7 +1354,7 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1368,7 +1362,7 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1376,7 +1370,7 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1384,7 +1378,7 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1392,7 +1386,7 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1400,7 +1394,7 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1408,7 +1402,7 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1416,7 +1410,7 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1424,7 +1418,7 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1432,7 +1426,7 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1440,7 +1434,7 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1448,7 +1442,7 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1456,7 +1450,7 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1464,7 +1458,7 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1472,7 +1466,7 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1480,7 +1474,7 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1488,7 +1482,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1496,7 +1490,7 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1504,7 +1498,7 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1512,7 +1506,7 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1520,7 +1514,7 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1528,7 +1522,7 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1536,7 +1530,7 @@
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1544,7 +1538,7 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1552,7 +1546,7 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1560,7 +1554,7 @@
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1568,7 +1562,7 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1576,7 +1570,7 @@
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1584,7 +1578,7 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1592,7 +1586,7 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1600,7 +1594,7 @@
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1608,7 +1602,7 @@
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1616,7 +1610,7 @@
         <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1624,7 +1618,7 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1632,7 +1626,7 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1640,7 +1634,7 @@
         <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1648,7 +1642,7 @@
         <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1656,7 +1650,7 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1664,7 +1658,7 @@
         <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1672,7 +1666,7 @@
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1680,7 +1674,7 @@
         <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1688,7 +1682,7 @@
         <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1696,7 +1690,7 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1704,7 +1698,7 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1712,7 +1706,7 @@
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1720,7 +1714,7 @@
         <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1728,7 +1722,7 @@
         <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1736,7 +1730,7 @@
         <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1744,7 +1738,7 @@
         <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1752,7 +1746,7 @@
         <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1760,7 +1754,7 @@
         <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1768,7 +1762,7 @@
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1776,7 +1770,7 @@
         <v>71</v>
       </c>
       <c r="B70" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1784,7 +1778,7 @@
         <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1792,7 +1786,7 @@
         <v>73</v>
       </c>
       <c r="B72" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1800,7 +1794,7 @@
         <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1808,7 +1802,7 @@
         <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1816,7 +1810,7 @@
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1824,7 +1818,7 @@
         <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1832,7 +1826,7 @@
         <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1840,7 +1834,7 @@
         <v>79</v>
       </c>
       <c r="B78" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1848,7 +1842,7 @@
         <v>80</v>
       </c>
       <c r="B79" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1856,7 +1850,7 @@
         <v>81</v>
       </c>
       <c r="B80" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1864,7 +1858,7 @@
         <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1872,7 +1866,7 @@
         <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1880,7 +1874,7 @@
         <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1888,7 +1882,7 @@
         <v>85</v>
       </c>
       <c r="B84" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -1896,7 +1890,7 @@
         <v>86</v>
       </c>
       <c r="B85" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1904,7 +1898,7 @@
         <v>87</v>
       </c>
       <c r="B86" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1912,7 +1906,7 @@
         <v>88</v>
       </c>
       <c r="B87" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -1920,7 +1914,7 @@
         <v>89</v>
       </c>
       <c r="B88" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -1928,7 +1922,7 @@
         <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1936,7 +1930,7 @@
         <v>91</v>
       </c>
       <c r="B90" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -1944,7 +1938,7 @@
         <v>92</v>
       </c>
       <c r="B91" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -1952,7 +1946,7 @@
         <v>93</v>
       </c>
       <c r="B92" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -1960,7 +1954,7 @@
         <v>94</v>
       </c>
       <c r="B93" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1968,7 +1962,7 @@
         <v>95</v>
       </c>
       <c r="B94" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -1976,7 +1970,7 @@
         <v>96</v>
       </c>
       <c r="B95" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -1984,7 +1978,7 @@
         <v>97</v>
       </c>
       <c r="B96" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -1992,7 +1986,7 @@
         <v>98</v>
       </c>
       <c r="B97" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -2000,7 +1994,7 @@
         <v>99</v>
       </c>
       <c r="B98" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -2008,7 +2002,7 @@
         <v>100</v>
       </c>
       <c r="B99" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -2016,7 +2010,7 @@
         <v>101</v>
       </c>
       <c r="B100" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -2024,7 +2018,7 @@
         <v>102</v>
       </c>
       <c r="B101" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -2032,7 +2026,7 @@
         <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -2040,7 +2034,7 @@
         <v>105</v>
       </c>
       <c r="B103" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -2048,7 +2042,7 @@
         <v>106</v>
       </c>
       <c r="B104" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -2056,7 +2050,7 @@
         <v>107</v>
       </c>
       <c r="B105" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -2064,7 +2058,7 @@
         <v>108</v>
       </c>
       <c r="B106" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -2072,7 +2066,7 @@
         <v>109</v>
       </c>
       <c r="B107" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -2080,7 +2074,7 @@
         <v>110</v>
       </c>
       <c r="B108" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -2088,7 +2082,7 @@
         <v>111</v>
       </c>
       <c r="B109" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -2096,7 +2090,7 @@
         <v>112</v>
       </c>
       <c r="B110" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -2104,7 +2098,7 @@
         <v>113</v>
       </c>
       <c r="B111" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -2112,7 +2106,7 @@
         <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -2120,7 +2114,7 @@
         <v>115</v>
       </c>
       <c r="B113" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -2128,7 +2122,7 @@
         <v>116</v>
       </c>
       <c r="B114" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -2136,7 +2130,7 @@
         <v>117</v>
       </c>
       <c r="B115" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -2144,7 +2138,7 @@
         <v>118</v>
       </c>
       <c r="B116" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -2152,7 +2146,7 @@
         <v>119</v>
       </c>
       <c r="B117" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -2160,7 +2154,7 @@
         <v>120</v>
       </c>
       <c r="B118" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -2168,7 +2162,7 @@
         <v>121</v>
       </c>
       <c r="B119" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -2176,7 +2170,7 @@
         <v>122</v>
       </c>
       <c r="B120" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -2184,7 +2178,7 @@
         <v>123</v>
       </c>
       <c r="B121" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -2192,7 +2186,7 @@
         <v>124</v>
       </c>
       <c r="B122" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -2200,7 +2194,7 @@
         <v>125</v>
       </c>
       <c r="B123" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -2208,7 +2202,7 @@
         <v>126</v>
       </c>
       <c r="B124" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -2216,7 +2210,7 @@
         <v>127</v>
       </c>
       <c r="B125" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -2224,7 +2218,7 @@
         <v>128</v>
       </c>
       <c r="B126" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -2232,7 +2226,7 @@
         <v>129</v>
       </c>
       <c r="B127" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -2240,7 +2234,7 @@
         <v>130</v>
       </c>
       <c r="B128" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -2248,7 +2242,7 @@
         <v>131</v>
       </c>
       <c r="B129" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -2256,7 +2250,7 @@
         <v>132</v>
       </c>
       <c r="B130" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -2264,7 +2258,7 @@
         <v>133</v>
       </c>
       <c r="B131" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -2272,7 +2266,7 @@
         <v>134</v>
       </c>
       <c r="B132" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -2280,7 +2274,7 @@
         <v>135</v>
       </c>
       <c r="B133" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -2288,7 +2282,7 @@
         <v>136</v>
       </c>
       <c r="B134" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -2296,15 +2290,7 @@
         <v>137</v>
       </c>
       <c r="B135" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>138</v>
-      </c>
-      <c r="B136" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>